<commit_message>
tutorial on food tree
</commit_message>
<xml_diff>
--- a/eg_data/VVKAJ/NOTES - diet lineplot.xlsx
+++ b/eg_data/VVKAJ/NOTES - diet lineplot.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\dietary_patterns\eg_data\VVKAJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187808DA-1E63-4925-969B-AD6153C8A1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31424A5-D65A-4D60-89E3-854F4A297123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21180" yWindow="-1815" windowWidth="17715" windowHeight="12510" xr2:uid="{F3F8738C-76B9-402C-9C92-B4067BFE35BA}"/>
+    <workbookView xWindow="29385" yWindow="-2865" windowWidth="18780" windowHeight="15390" activeTab="2" xr2:uid="{F3F8738C-76B9-402C-9C92-B4067BFE35BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="PCA order" sheetId="2" r:id="rId2"/>
-    <sheet name="catasis" sheetId="3" r:id="rId3"/>
+    <sheet name="cat asis" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2487,7 +2487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C0559A-7669-47BF-BFBD-62D762233AAD}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3538,7 +3538,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D27"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3930,11 +3930,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1ACBBC-88F5-474F-90F9-2221112C409E}">
   <dimension ref="A1:EH27"/>
   <sheetViews>
-    <sheetView topLeftCell="DH1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="112" max="112" width="8.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:138" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>